<commit_message>
Theme of files updated, tests modified to fit new names, cards and characters text files added
</commit_message>
<xml_diff>
--- a/Board.xlsx
+++ b/Board.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\timmy_000\Documents\CSM\Spring 2015\software engineering\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145"/>
   </bookViews>
@@ -32,39 +27,15 @@
     <t>R</t>
   </si>
   <si>
-    <t>S</t>
-  </si>
-  <si>
     <t>X</t>
   </si>
   <si>
-    <t>H</t>
-  </si>
-  <si>
     <t>B</t>
   </si>
   <si>
-    <t>K</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>O</t>
-  </si>
-  <si>
     <t>L</t>
   </si>
   <si>
-    <t>LD</t>
-  </si>
-  <si>
-    <t>HL</t>
-  </si>
-  <si>
-    <t>RD</t>
-  </si>
-  <si>
     <t>RL</t>
   </si>
   <si>
@@ -77,69 +48,15 @@
     <t>BR</t>
   </si>
   <si>
-    <t>KU</t>
-  </si>
-  <si>
-    <t>KR</t>
-  </si>
-  <si>
-    <t>DR</t>
-  </si>
-  <si>
-    <t>OL</t>
-  </si>
-  <si>
-    <t>OU</t>
-  </si>
-  <si>
-    <t>SD</t>
-  </si>
-  <si>
-    <t>SL</t>
-  </si>
-  <si>
     <t>LR</t>
   </si>
   <si>
     <t>RR</t>
   </si>
   <si>
-    <t>Cat Room</t>
-  </si>
-  <si>
-    <t>Loomery</t>
-  </si>
-  <si>
-    <t>Sauna</t>
-  </si>
-  <si>
-    <t>Halfway House</t>
-  </si>
-  <si>
-    <t>Dog Room</t>
-  </si>
-  <si>
-    <t>CL</t>
-  </si>
-  <si>
-    <t>DD</t>
-  </si>
-  <si>
-    <t>Ballad Room</t>
-  </si>
-  <si>
-    <t>Kaligraphy Room</t>
-  </si>
-  <si>
     <t>Walkway</t>
   </si>
   <si>
-    <t>Bob</t>
-  </si>
-  <si>
-    <t>Room</t>
-  </si>
-  <si>
     <t>Brown: walkway scenarios</t>
   </si>
   <si>
@@ -156,6 +73,84 @@
   </si>
   <si>
     <t>Green: Beside Wall</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>ML</t>
+  </si>
+  <si>
+    <t>MU</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>FL</t>
+  </si>
+  <si>
+    <t>LU</t>
+  </si>
+  <si>
+    <t>CD</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>NR</t>
+  </si>
+  <si>
+    <t>ND</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>TR</t>
+  </si>
+  <si>
+    <t>TD</t>
+  </si>
+  <si>
+    <t>TL</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>AL</t>
+  </si>
+  <si>
+    <t>AD</t>
+  </si>
+  <si>
+    <t>MacLaren's Pub</t>
+  </si>
+  <si>
+    <t>Barney's Bachelor Pad</t>
+  </si>
+  <si>
+    <t>Ted's Apartment</t>
+  </si>
+  <si>
+    <t>Laser Tag Arena</t>
+  </si>
+  <si>
+    <t>The Captain's Boat</t>
+  </si>
+  <si>
+    <t>Lily's Classroom</t>
+  </si>
+  <si>
+    <t>Metro News 1</t>
+  </si>
+  <si>
+    <t>Cafe L'amour</t>
+  </si>
+  <si>
+    <t>Farhampton Inn</t>
   </si>
 </sst>
 </file>
@@ -275,35 +270,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Style 1" xfId="7"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill>
@@ -367,7 +334,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -402,7 +369,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -614,7 +581,7 @@
   <dimension ref="A1:AB37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AB25" sqref="AB25"/>
+      <selection activeCell="AB15" sqref="AB15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -625,19 +592,19 @@
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="D1" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="E1" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="F1" s="7" t="s">
         <v>1</v>
@@ -646,37 +613,37 @@
         <v>1</v>
       </c>
       <c r="H1" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="I1" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="J1" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="K1" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="L1" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="M1" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="N1" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="O1" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="P1" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="Q1" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="R1" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="S1" s="7" t="s">
         <v>1</v>
@@ -685,10 +652,10 @@
         <v>1</v>
       </c>
       <c r="U1" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="V1" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="W1">
         <v>0</v>
@@ -696,19 +663,19 @@
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>1</v>
@@ -717,37 +684,37 @@
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="I2" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="J2" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="K2" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="L2" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="M2" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="N2" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="O2" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="P2" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="Q2" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="S2" s="7" t="s">
         <v>1</v>
@@ -756,10 +723,10 @@
         <v>1</v>
       </c>
       <c r="U2" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="V2" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="W2">
         <v>1</v>
@@ -767,19 +734,19 @@
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>1</v>
@@ -788,37 +755,37 @@
         <v>1</v>
       </c>
       <c r="H3" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="I3" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="J3" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="K3" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="L3" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="M3" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="N3" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="O3" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="P3" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="Q3" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="R3" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="S3" s="7" t="s">
         <v>1</v>
@@ -827,10 +794,10 @@
         <v>1</v>
       </c>
       <c r="U3" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="V3" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="W3">
         <v>2</v>
@@ -838,19 +805,19 @@
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="E4" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="F4" s="7" t="s">
         <v>1</v>
@@ -859,22 +826,22 @@
         <v>1</v>
       </c>
       <c r="H4" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="I4" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="J4" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="K4" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="L4" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="M4" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="N4" s="7" t="s">
         <v>1</v>
@@ -898,36 +865,36 @@
         <v>1</v>
       </c>
       <c r="U4" s="4" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="V4" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="W4">
         <v>3</v>
       </c>
       <c r="AA4" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="AB4" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>1</v>
@@ -936,22 +903,22 @@
         <v>1</v>
       </c>
       <c r="H5" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="I5" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="J5" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="K5" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="L5" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="M5" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="N5" s="7" t="s">
         <v>1</v>
@@ -975,36 +942,36 @@
         <v>1</v>
       </c>
       <c r="U5" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="V5" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="W5">
         <v>4</v>
       </c>
       <c r="AA5" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AB5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F6" s="7" t="s">
         <v>1</v>
@@ -1013,34 +980,34 @@
         <v>1</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="I6" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="J6" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="K6" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="L6" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="N6" s="7" t="s">
         <v>1</v>
       </c>
       <c r="O6" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="P6" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="R6" s="7" t="s">
         <v>1</v>
@@ -1052,36 +1019,36 @@
         <v>1</v>
       </c>
       <c r="U6" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="V6" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="W6">
         <v>5</v>
       </c>
       <c r="AA6" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="AB6" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="E7" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>1</v>
@@ -1111,13 +1078,13 @@
         <v>1</v>
       </c>
       <c r="O7" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="P7" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="Q7" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="R7" s="7" t="s">
         <v>1</v>
@@ -1129,36 +1096,36 @@
         <v>1</v>
       </c>
       <c r="U7" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="V7" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="W7">
         <v>6</v>
       </c>
       <c r="AA7" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AB7" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="D8" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="E8" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="F8" s="7" t="s">
         <v>1</v>
@@ -1188,13 +1155,13 @@
         <v>1</v>
       </c>
       <c r="O8" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="P8" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="Q8" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="R8" s="7" t="s">
         <v>1</v>
@@ -1206,96 +1173,96 @@
         <v>1</v>
       </c>
       <c r="U8" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="V8" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="W8">
         <v>7</v>
       </c>
       <c r="AA8" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AB8" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="D9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="L9" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="M9" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="N9" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="O9" t="s">
+        <v>0</v>
+      </c>
+      <c r="P9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>0</v>
+      </c>
+      <c r="R9" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="S9" t="s">
         <v>33</v>
       </c>
-      <c r="E9" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="I9" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="J9" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="K9" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="L9" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="M9" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="N9" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="O9" t="s">
-        <v>10</v>
-      </c>
-      <c r="P9" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>10</v>
-      </c>
-      <c r="R9" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="S9" t="s">
-        <v>3</v>
-      </c>
       <c r="T9" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="U9" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="V9" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="W9">
         <v>8</v>
       </c>
       <c r="AA9" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="AB9" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
@@ -1354,25 +1321,25 @@
         <v>1</v>
       </c>
       <c r="S10" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="T10" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="U10" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="V10" s="2" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="W10">
         <v>9</v>
       </c>
       <c r="AA10" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="AB10" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.25">
@@ -1398,25 +1365,25 @@
         <v>1</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O11" s="7" t="s">
         <v>1</v>
@@ -1446,10 +1413,10 @@
         <v>10</v>
       </c>
       <c r="AA11" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="AB11" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.25">
@@ -1475,25 +1442,25 @@
         <v>1</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O12" s="7" t="s">
         <v>1</v>
@@ -1505,45 +1472,45 @@
         <v>1</v>
       </c>
       <c r="R12" s="2" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="S12" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="T12" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="U12" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="V12" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="W12">
         <v>11</v>
       </c>
       <c r="AA12" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="AB12" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="E13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F13" s="7" t="s">
         <v>1</v>
@@ -1552,25 +1519,25 @@
         <v>1</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O13" s="7" t="s">
         <v>1</v>
@@ -1582,19 +1549,19 @@
         <v>1</v>
       </c>
       <c r="R13" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="S13" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="T13" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="U13" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="V13" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="W13">
         <v>12</v>
@@ -1603,24 +1570,24 @@
         <v>1</v>
       </c>
       <c r="AB13" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F14" s="7" t="s">
         <v>1</v>
@@ -1629,25 +1596,25 @@
         <v>1</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O14" s="7" t="s">
         <v>1</v>
@@ -1659,19 +1626,19 @@
         <v>1</v>
       </c>
       <c r="R14" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="S14" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="T14" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="U14" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="V14" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="W14">
         <v>13</v>
@@ -1679,19 +1646,19 @@
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F15" s="7" t="s">
         <v>1</v>
@@ -1700,25 +1667,25 @@
         <v>1</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O15" s="7" t="s">
         <v>1</v>
@@ -1730,19 +1697,19 @@
         <v>1</v>
       </c>
       <c r="R15" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="S15" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="T15" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="U15" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="V15" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="W15">
         <v>14</v>
@@ -1750,19 +1717,19 @@
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F16" s="7" t="s">
         <v>1</v>
@@ -1771,25 +1738,25 @@
         <v>1</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O16" s="7" t="s">
         <v>1</v>
@@ -1801,19 +1768,19 @@
         <v>1</v>
       </c>
       <c r="R16" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="S16" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="T16" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="U16" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="V16" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="W16">
         <v>15</v>
@@ -1821,19 +1788,19 @@
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B17" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D17" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E17" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F17" s="7" t="s">
         <v>1</v>
@@ -1842,25 +1809,25 @@
         <v>1</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O17" s="7" t="s">
         <v>1</v>
@@ -1872,19 +1839,19 @@
         <v>1</v>
       </c>
       <c r="R17" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="S17" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="T17" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="U17" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="V17" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="W17">
         <v>16</v>
@@ -1892,19 +1859,19 @@
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B18" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C18" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E18" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F18" s="7" t="s">
         <v>1</v>
@@ -1913,25 +1880,25 @@
         <v>1</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O18" s="7" t="s">
         <v>1</v>
@@ -1943,19 +1910,19 @@
         <v>1</v>
       </c>
       <c r="R18" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="S18" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="T18" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="U18" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="V18" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="W18">
         <v>17</v>
@@ -1963,19 +1930,19 @@
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B19" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C19" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D19" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E19" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F19" s="7" t="s">
         <v>1</v>
@@ -1984,25 +1951,25 @@
         <v>1</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O19" s="7" t="s">
         <v>1</v>
@@ -2014,19 +1981,19 @@
         <v>1</v>
       </c>
       <c r="R19" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="S19" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="T19" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="U19" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="V19" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="W19">
         <v>18</v>
@@ -2034,19 +2001,19 @@
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B20" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C20" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D20" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E20" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F20" s="7" t="s">
         <v>1</v>
@@ -2085,19 +2052,19 @@
         <v>1</v>
       </c>
       <c r="R20" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="S20" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="T20" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="U20" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="V20" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="W20">
         <v>19</v>
@@ -2105,19 +2072,19 @@
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B21" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D21" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E21" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F21" s="7" t="s">
         <v>1</v>
@@ -2156,19 +2123,19 @@
         <v>1</v>
       </c>
       <c r="R21" s="2" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="S21" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="T21" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="U21" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="V21" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="W21">
         <v>20</v>
@@ -2176,19 +2143,19 @@
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B22" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C22" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D22" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F22" s="7" t="s">
         <v>1</v>
@@ -2268,10 +2235,10 @@
         <v>1</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="J23" s="7" t="s">
         <v>1</v>
@@ -2280,37 +2247,37 @@
         <v>1</v>
       </c>
       <c r="L23" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M23" t="s">
+        <v>19</v>
+      </c>
+      <c r="N23" t="s">
+        <v>19</v>
+      </c>
+      <c r="O23" t="s">
+        <v>19</v>
+      </c>
+      <c r="P23" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>19</v>
+      </c>
+      <c r="R23" t="s">
+        <v>19</v>
+      </c>
+      <c r="S23" t="s">
+        <v>19</v>
+      </c>
+      <c r="T23" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="M23" t="s">
-        <v>9</v>
-      </c>
-      <c r="N23" t="s">
-        <v>9</v>
-      </c>
-      <c r="O23" t="s">
-        <v>9</v>
-      </c>
-      <c r="P23" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>9</v>
-      </c>
-      <c r="R23" t="s">
-        <v>9</v>
-      </c>
-      <c r="S23" t="s">
-        <v>9</v>
-      </c>
-      <c r="T23" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="U23" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="V23" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="W23">
         <v>22</v>
@@ -2318,19 +2285,19 @@
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="B24" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C24" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D24" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E24" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F24" s="7" t="s">
         <v>1</v>
@@ -2339,10 +2306,10 @@
         <v>1</v>
       </c>
       <c r="H24" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I24" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J24" s="7" t="s">
         <v>1</v>
@@ -2351,37 +2318,37 @@
         <v>1</v>
       </c>
       <c r="L24" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="M24" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="N24" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="O24" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="P24" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="Q24" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="R24" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="S24" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="T24" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="U24" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="V24" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="W24">
         <v>23</v>
@@ -2389,19 +2356,19 @@
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B25" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C25" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D25" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E25" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F25" s="7" t="s">
         <v>1</v>
@@ -2410,10 +2377,10 @@
         <v>1</v>
       </c>
       <c r="H25" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I25" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J25" s="7" t="s">
         <v>1</v>
@@ -2422,37 +2389,37 @@
         <v>1</v>
       </c>
       <c r="L25" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="M25" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="N25" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="O25" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="P25" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="Q25" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="R25" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="S25" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="T25" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="U25" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="V25" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="W25">
         <v>24</v>
@@ -2460,19 +2427,19 @@
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B26" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C26" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D26" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E26" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F26" s="7" t="s">
         <v>1</v>
@@ -2481,10 +2448,10 @@
         <v>1</v>
       </c>
       <c r="H26" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I26" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J26" s="7" t="s">
         <v>1</v>
@@ -2493,37 +2460,37 @@
         <v>1</v>
       </c>
       <c r="L26" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="M26" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="N26" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="O26" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="P26" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="Q26" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="R26" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="S26" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="T26" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="U26" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="V26" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="W26">
         <v>25</v>
@@ -2531,19 +2498,19 @@
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B27" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C27" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D27" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E27" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F27" s="7" t="s">
         <v>1</v>
@@ -2552,10 +2519,10 @@
         <v>1</v>
       </c>
       <c r="H27" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I27" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J27" s="7" t="s">
         <v>1</v>
@@ -2564,37 +2531,37 @@
         <v>1</v>
       </c>
       <c r="L27" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="M27" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="N27" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="O27" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="P27" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="Q27" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="R27" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="S27" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="T27" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="U27" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="V27" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="W27">
         <v>26</v>
@@ -2602,19 +2569,19 @@
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B28" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C28" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D28" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="F28" s="7" t="s">
         <v>1</v>
@@ -2623,10 +2590,10 @@
         <v>1</v>
       </c>
       <c r="H28" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I28" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J28" s="7" t="s">
         <v>1</v>
@@ -2635,37 +2602,37 @@
         <v>1</v>
       </c>
       <c r="L28" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="M28" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="N28" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="O28" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="P28" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="Q28" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="R28" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="S28" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="T28" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="U28" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="V28" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="W28">
         <v>27</v>
@@ -2741,37 +2708,37 @@
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>40</v>
+        <v>14</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>42</v>
+        <v>16</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="Y23">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>"W"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>